<commit_message>
Resolved merged conflicts & added Medical records xlsx
</commit_message>
<xml_diff>
--- a/data/MedicalRecordList.xlsx
+++ b/data/MedicalRecordList.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>test123@gmail.com</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
         <v>8.7654321E7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Added Appointment List Excel & Finished View Available Appointments
</commit_message>
<xml_diff>
--- a/data/MedicalRecordList.xlsx
+++ b/data/MedicalRecordList.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2dc85ffdfb189c0/Desktop/School Projects/SC2002 - OBJECT ORIENTIATED DESIGN ^0 PROGRAMMING/OOP_Proj/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A930262-F376-4236-B3A1-ECC5AC40F227}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B61270C7-1DE0-43F6-81D7-7C8D8400AF34}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Past Dianoses &amp; Treatments</t>
   </si>
   <si>
-    <t>P001</t>
-  </si>
-  <si>
     <t>MR001</t>
   </si>
   <si>
@@ -66,27 +63,15 @@
     <t>Male</t>
   </si>
   <si>
-    <t>user1@example.com</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua.</t>
-  </si>
-  <si>
     <t>12-08-1999</t>
   </si>
   <si>
     <t>MR002</t>
   </si>
   <si>
-    <t>P003</t>
-  </si>
-  <si>
-    <t>User3</t>
-  </si>
-  <si>
     <t>18-02-1998</t>
   </si>
   <si>
@@ -96,20 +81,31 @@
     <t>B</t>
   </si>
   <si>
-    <t>test123@gmail.com</t>
-  </si>
-  <si>
-    <t>12345678</t>
-  </si>
-  <si>
     <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>H005</t>
+  </si>
+  <si>
+    <t>H025</t>
+  </si>
+  <si>
+    <t>User21</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Winter is coming</t>
+  </si>
+  <si>
+    <t>Fire and Blood</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,20 +469,20 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.36328125"/>
-    <col min="2" max="2" customWidth="true" width="14.6328125"/>
-    <col min="3" max="3" customWidth="true" width="11.6328125"/>
-    <col min="4" max="4" customWidth="true" width="11.36328125"/>
-    <col min="5" max="5" customWidth="true" width="12.26953125"/>
-    <col min="6" max="6" customWidth="true" width="14.6328125"/>
-    <col min="7" max="7" customWidth="true" width="20.6328125"/>
-    <col min="8" max="8" customWidth="true" width="14.7265625"/>
-    <col min="9" max="9" customWidth="true" width="31.90625"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="31.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -520,60 +516,60 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2">
+        <v>87654321</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>8.7654321E7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2">
         <v>9853249</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove past diagnoses column from medical record excel
</commit_message>
<xml_diff>
--- a/data/MedicalRecordList.xlsx
+++ b/data/MedicalRecordList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2dc85ffdfb189c0/Desktop/School Projects/SC2002 - OBJECT ORIENTIATED DESIGN ^0 PROGRAMMING/OOP_Proj/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharon\Documents\NTU\NTU\Y2\OODP\OOP_Proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B61270C7-1DE0-43F6-81D7-7C8D8400AF34}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2956D0A-9257-44E4-A4E8-74256E718636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Blood Type</t>
   </si>
   <si>
-    <t>Past Dianoses &amp; Treatments</t>
-  </si>
-  <si>
     <t>MR001</t>
   </si>
   <si>
@@ -94,12 +91,6 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>Winter is coming</t>
-  </si>
-  <si>
-    <t>Fire and Blood</t>
   </si>
 </sst>
 </file>
@@ -197,10 +188,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,10 +469,9 @@
     <col min="6" max="6" width="14.6328125" customWidth="1"/>
     <col min="7" max="7" width="20.6328125" customWidth="1"/>
     <col min="8" max="8" width="14.7265625" customWidth="1"/>
-    <col min="9" max="9" width="31.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -510,66 +496,57 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="2">
         <v>87654321</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="2">
         <v>9853249</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>